<commit_message>
Add conditions for each participant
</commit_message>
<xml_diff>
--- a/script/Max/cb.xlsx
+++ b/script/Max/cb.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsukotominaga/Dropbox (Personal)/- Research/[Project]/GitHub/expert01/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsukotominaga/OneDrive - Central European University/Project/ExpertTeaching/script/Max/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18254B6C-6F0E-484E-BE8D-5C91567D5B9D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{18254B6C-6F0E-484E-BE8D-5C91567D5B9D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{267F4345-77DB-F84C-8E0D-21DD56B71286}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{52DF1984-8799-084D-A002-69ECD2D6256B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="19">
   <si>
     <t>;</t>
   </si>
@@ -64,6 +64,24 @@
   </si>
   <si>
     <t>t_e1</t>
+  </si>
+  <si>
+    <t>firstCond</t>
+  </si>
+  <si>
+    <t>firstScore</t>
+  </si>
+  <si>
+    <t>secondScore</t>
+  </si>
+  <si>
+    <t>Teaching</t>
+  </si>
+  <si>
+    <t>Performing</t>
+  </si>
+  <si>
+    <t>secondCond</t>
   </si>
 </sst>
 </file>
@@ -415,387 +433,511 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F79E29-5F9D-CD42-974F-D0505AEE028B}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="A2:E9"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>0</v>
       </c>
-      <c r="H2" t="str">
-        <f>CONCATENATE(A2,F2)</f>
+      <c r="J2" t="str">
+        <f>CONCATENATE(A2,H2)</f>
         <v>1,</v>
       </c>
-      <c r="I2" t="str">
+      <c r="K2" t="str">
         <f>B2</f>
+        <v>Teaching</v>
+      </c>
+      <c r="L2" t="str">
+        <f>C2</f>
+        <v>Performing</v>
+      </c>
+      <c r="M2" t="str">
+        <f>D2</f>
         <v>articulation</v>
       </c>
-      <c r="J2" t="str">
-        <f>C2</f>
+      <c r="N2" t="str">
+        <f>E2</f>
         <v>tempoChange</v>
       </c>
-      <c r="K2" t="str">
-        <f>D2</f>
+      <c r="O2" t="str">
+        <f>F2</f>
         <v>a_e1</v>
       </c>
-      <c r="L2" t="str">
-        <f>CONCATENATE(E2,G2)</f>
+      <c r="P2" t="str">
+        <f>CONCATENATE(G2,I2)</f>
         <v>t_e2;</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>0</v>
       </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H9" si="0">CONCATENATE(A3,F3)</f>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J9" si="0">CONCATENATE(A3,H3)</f>
         <v>2,</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I9" si="1">B3</f>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K9" si="1">B3</f>
+        <v>Performing</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L9" si="2">C3</f>
+        <v>Teaching</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M9" si="3">D3</f>
         <v>articulation</v>
       </c>
-      <c r="J3" t="str">
-        <f t="shared" ref="J3:J9" si="2">C3</f>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N9" si="4">E3</f>
         <v>tempoChange</v>
       </c>
-      <c r="K3" t="str">
-        <f t="shared" ref="K3:K9" si="3">D3</f>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O9" si="5">F3</f>
         <v>a_e1</v>
       </c>
-      <c r="L3" t="str">
-        <f t="shared" ref="L3:L9" si="4">CONCATENATE(E3,G3)</f>
+      <c r="P3" t="str">
+        <f t="shared" ref="P3:P9" si="6">CONCATENATE(G3,I3)</f>
         <v>t_e2;</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>0</v>
       </c>
-      <c r="H4" t="str">
+      <c r="J4" t="str">
         <f t="shared" si="0"/>
         <v>3,</v>
       </c>
-      <c r="I4" t="str">
+      <c r="K4" t="str">
         <f t="shared" si="1"/>
+        <v>Teaching</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="2"/>
+        <v>Performing</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="3"/>
         <v>articulation</v>
       </c>
-      <c r="J4" t="str">
-        <f t="shared" si="2"/>
+      <c r="N4" t="str">
+        <f t="shared" si="4"/>
         <v>tempoChange</v>
       </c>
-      <c r="K4" t="str">
-        <f t="shared" si="3"/>
+      <c r="O4" t="str">
+        <f t="shared" si="5"/>
         <v>a_e2</v>
       </c>
-      <c r="L4" t="str">
-        <f t="shared" si="4"/>
+      <c r="P4" t="str">
+        <f t="shared" si="6"/>
         <v>t_e1;</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>0</v>
       </c>
-      <c r="H5" t="str">
+      <c r="J5" t="str">
         <f t="shared" si="0"/>
         <v>4,</v>
       </c>
-      <c r="I5" t="str">
+      <c r="K5" t="str">
         <f t="shared" si="1"/>
+        <v>Performing</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="2"/>
+        <v>Teaching</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="3"/>
         <v>articulation</v>
       </c>
-      <c r="J5" t="str">
-        <f t="shared" si="2"/>
+      <c r="N5" t="str">
+        <f t="shared" si="4"/>
         <v>tempoChange</v>
       </c>
-      <c r="K5" t="str">
-        <f t="shared" si="3"/>
+      <c r="O5" t="str">
+        <f t="shared" si="5"/>
         <v>a_e2</v>
       </c>
-      <c r="L5" t="str">
-        <f t="shared" si="4"/>
+      <c r="P5" t="str">
+        <f t="shared" si="6"/>
         <v>t_e1;</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>0</v>
       </c>
-      <c r="H6" t="str">
+      <c r="J6" t="str">
         <f t="shared" si="0"/>
         <v>5,</v>
       </c>
-      <c r="I6" t="str">
+      <c r="K6" t="str">
         <f t="shared" si="1"/>
+        <v>Teaching</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="2"/>
+        <v>Performing</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="3"/>
         <v>tempoChange</v>
       </c>
-      <c r="J6" t="str">
-        <f t="shared" si="2"/>
+      <c r="N6" t="str">
+        <f t="shared" si="4"/>
         <v>articulation</v>
       </c>
-      <c r="K6" t="str">
-        <f t="shared" si="3"/>
+      <c r="O6" t="str">
+        <f t="shared" si="5"/>
         <v>t_e1</v>
       </c>
-      <c r="L6" t="str">
-        <f t="shared" si="4"/>
+      <c r="P6" t="str">
+        <f t="shared" si="6"/>
         <v>a_e2;</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>1</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>0</v>
       </c>
-      <c r="H7" t="str">
+      <c r="J7" t="str">
         <f t="shared" si="0"/>
         <v>6,</v>
       </c>
-      <c r="I7" t="str">
+      <c r="K7" t="str">
         <f t="shared" si="1"/>
+        <v>Performing</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="2"/>
+        <v>Teaching</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="3"/>
         <v>tempoChange</v>
       </c>
-      <c r="J7" t="str">
-        <f t="shared" si="2"/>
+      <c r="N7" t="str">
+        <f t="shared" si="4"/>
         <v>articulation</v>
       </c>
-      <c r="K7" t="str">
-        <f t="shared" si="3"/>
+      <c r="O7" t="str">
+        <f t="shared" si="5"/>
         <v>t_e1</v>
       </c>
-      <c r="L7" t="str">
-        <f t="shared" si="4"/>
+      <c r="P7" t="str">
+        <f t="shared" si="6"/>
         <v>a_e2;</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>9</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>1</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>0</v>
       </c>
-      <c r="H8" t="str">
+      <c r="J8" t="str">
         <f t="shared" si="0"/>
         <v>7,</v>
       </c>
-      <c r="I8" t="str">
+      <c r="K8" t="str">
         <f t="shared" si="1"/>
+        <v>Teaching</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="2"/>
+        <v>Performing</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="3"/>
         <v>tempoChange</v>
       </c>
-      <c r="J8" t="str">
-        <f t="shared" si="2"/>
+      <c r="N8" t="str">
+        <f t="shared" si="4"/>
         <v>articulation</v>
       </c>
-      <c r="K8" t="str">
-        <f t="shared" si="3"/>
+      <c r="O8" t="str">
+        <f t="shared" si="5"/>
         <v>t_e2</v>
       </c>
-      <c r="L8" t="str">
-        <f t="shared" si="4"/>
+      <c r="P8" t="str">
+        <f t="shared" si="6"/>
         <v>a_e1;</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>0</v>
       </c>
-      <c r="H9" t="str">
+      <c r="J9" t="str">
         <f t="shared" si="0"/>
         <v>8,</v>
       </c>
-      <c r="I9" t="str">
+      <c r="K9" t="str">
         <f t="shared" si="1"/>
+        <v>Performing</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="2"/>
+        <v>Teaching</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="3"/>
         <v>tempoChange</v>
       </c>
-      <c r="J9" t="str">
-        <f t="shared" si="2"/>
+      <c r="N9" t="str">
+        <f t="shared" si="4"/>
         <v>articulation</v>
       </c>
-      <c r="K9" t="str">
-        <f t="shared" si="3"/>
+      <c r="O9" t="str">
+        <f t="shared" si="5"/>
         <v>t_e2</v>
       </c>
-      <c r="L9" t="str">
-        <f t="shared" si="4"/>
+      <c r="P9" t="str">
+        <f t="shared" si="6"/>
         <v>a_e1;</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Add conditions for each participant"
This reverts commit e2dda3eca743d764c4539424e9bcb3a452bffe2b.
</commit_message>
<xml_diff>
--- a/script/Max/cb.xlsx
+++ b/script/Max/cb.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsukotominaga/OneDrive - Central European University/Project/ExpertTeaching/script/Max/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsukotominaga/Dropbox (Personal)/- Research/[Project]/GitHub/expert01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{18254B6C-6F0E-484E-BE8D-5C91567D5B9D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{267F4345-77DB-F84C-8E0D-21DD56B71286}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18254B6C-6F0E-484E-BE8D-5C91567D5B9D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{52DF1984-8799-084D-A002-69ECD2D6256B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="13">
   <si>
     <t>;</t>
   </si>
@@ -64,24 +64,6 @@
   </si>
   <si>
     <t>t_e1</t>
-  </si>
-  <si>
-    <t>firstCond</t>
-  </si>
-  <si>
-    <t>firstScore</t>
-  </si>
-  <si>
-    <t>secondScore</t>
-  </si>
-  <si>
-    <t>Teaching</t>
-  </si>
-  <si>
-    <t>Performing</t>
-  </si>
-  <si>
-    <t>secondCond</t>
   </si>
 </sst>
 </file>
@@ -433,511 +415,387 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F79E29-5F9D-CD42-974F-D0505AEE028B}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="E9" sqref="A2:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
       <c r="K1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
         <v>0</v>
       </c>
+      <c r="H2" t="str">
+        <f>CONCATENATE(A2,F2)</f>
+        <v>1,</v>
+      </c>
+      <c r="I2" t="str">
+        <f>B2</f>
+        <v>articulation</v>
+      </c>
       <c r="J2" t="str">
-        <f>CONCATENATE(A2,H2)</f>
-        <v>1,</v>
+        <f>C2</f>
+        <v>tempoChange</v>
       </c>
       <c r="K2" t="str">
-        <f>B2</f>
-        <v>Teaching</v>
+        <f>D2</f>
+        <v>a_e1</v>
       </c>
       <c r="L2" t="str">
-        <f>C2</f>
-        <v>Performing</v>
-      </c>
-      <c r="M2" t="str">
-        <f>D2</f>
-        <v>articulation</v>
-      </c>
-      <c r="N2" t="str">
-        <f>E2</f>
-        <v>tempoChange</v>
-      </c>
-      <c r="O2" t="str">
-        <f>F2</f>
-        <v>a_e1</v>
-      </c>
-      <c r="P2" t="str">
-        <f>CONCATENATE(G2,I2)</f>
+        <f>CONCATENATE(E2,G2)</f>
         <v>t_e2;</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
         <v>0</v>
       </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H9" si="0">CONCATENATE(A3,F3)</f>
+        <v>2,</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I9" si="1">B3</f>
+        <v>articulation</v>
+      </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J9" si="0">CONCATENATE(A3,H3)</f>
-        <v>2,</v>
+        <f t="shared" ref="J3:J9" si="2">C3</f>
+        <v>tempoChange</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K9" si="1">B3</f>
-        <v>Performing</v>
+        <f t="shared" ref="K3:K9" si="3">D3</f>
+        <v>a_e1</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L9" si="2">C3</f>
-        <v>Teaching</v>
-      </c>
-      <c r="M3" t="str">
-        <f t="shared" ref="M3:M9" si="3">D3</f>
-        <v>articulation</v>
-      </c>
-      <c r="N3" t="str">
-        <f t="shared" ref="N3:N9" si="4">E3</f>
-        <v>tempoChange</v>
-      </c>
-      <c r="O3" t="str">
-        <f t="shared" ref="O3:O9" si="5">F3</f>
-        <v>a_e1</v>
-      </c>
-      <c r="P3" t="str">
-        <f t="shared" ref="P3:P9" si="6">CONCATENATE(G3,I3)</f>
+        <f t="shared" ref="L3:L9" si="4">CONCATENATE(E3,G3)</f>
         <v>t_e2;</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
         <v>0</v>
       </c>
-      <c r="J4" t="str">
+      <c r="H4" t="str">
         <f t="shared" si="0"/>
         <v>3,</v>
       </c>
+      <c r="I4" t="str">
+        <f t="shared" si="1"/>
+        <v>articulation</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="2"/>
+        <v>tempoChange</v>
+      </c>
       <c r="K4" t="str">
-        <f t="shared" si="1"/>
-        <v>Teaching</v>
+        <f t="shared" si="3"/>
+        <v>a_e2</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" si="2"/>
-        <v>Performing</v>
-      </c>
-      <c r="M4" t="str">
-        <f t="shared" si="3"/>
-        <v>articulation</v>
-      </c>
-      <c r="N4" t="str">
         <f t="shared" si="4"/>
-        <v>tempoChange</v>
-      </c>
-      <c r="O4" t="str">
-        <f t="shared" si="5"/>
-        <v>a_e2</v>
-      </c>
-      <c r="P4" t="str">
-        <f t="shared" si="6"/>
         <v>t_e1;</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
         <v>0</v>
       </c>
-      <c r="J5" t="str">
+      <c r="H5" t="str">
         <f t="shared" si="0"/>
         <v>4,</v>
       </c>
+      <c r="I5" t="str">
+        <f t="shared" si="1"/>
+        <v>articulation</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="2"/>
+        <v>tempoChange</v>
+      </c>
       <c r="K5" t="str">
-        <f t="shared" si="1"/>
-        <v>Performing</v>
+        <f t="shared" si="3"/>
+        <v>a_e2</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="2"/>
-        <v>Teaching</v>
-      </c>
-      <c r="M5" t="str">
-        <f t="shared" si="3"/>
-        <v>articulation</v>
-      </c>
-      <c r="N5" t="str">
         <f t="shared" si="4"/>
-        <v>tempoChange</v>
-      </c>
-      <c r="O5" t="str">
-        <f t="shared" si="5"/>
-        <v>a_e2</v>
-      </c>
-      <c r="P5" t="str">
-        <f t="shared" si="6"/>
         <v>t_e1;</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
         <v>0</v>
       </c>
-      <c r="J6" t="str">
+      <c r="H6" t="str">
         <f t="shared" si="0"/>
         <v>5,</v>
       </c>
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v>tempoChange</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="2"/>
+        <v>articulation</v>
+      </c>
       <c r="K6" t="str">
-        <f t="shared" si="1"/>
-        <v>Teaching</v>
+        <f t="shared" si="3"/>
+        <v>t_e1</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="2"/>
-        <v>Performing</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" si="3"/>
-        <v>tempoChange</v>
-      </c>
-      <c r="N6" t="str">
         <f t="shared" si="4"/>
-        <v>articulation</v>
-      </c>
-      <c r="O6" t="str">
-        <f t="shared" si="5"/>
-        <v>t_e1</v>
-      </c>
-      <c r="P6" t="str">
-        <f t="shared" si="6"/>
         <v>a_e2;</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
         <v>0</v>
       </c>
-      <c r="J7" t="str">
+      <c r="H7" t="str">
         <f t="shared" si="0"/>
         <v>6,</v>
       </c>
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v>tempoChange</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="2"/>
+        <v>articulation</v>
+      </c>
       <c r="K7" t="str">
-        <f t="shared" si="1"/>
-        <v>Performing</v>
+        <f t="shared" si="3"/>
+        <v>t_e1</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="2"/>
-        <v>Teaching</v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" si="3"/>
-        <v>tempoChange</v>
-      </c>
-      <c r="N7" t="str">
         <f t="shared" si="4"/>
-        <v>articulation</v>
-      </c>
-      <c r="O7" t="str">
-        <f t="shared" si="5"/>
-        <v>t_e1</v>
-      </c>
-      <c r="P7" t="str">
-        <f t="shared" si="6"/>
         <v>a_e2;</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
         <v>0</v>
       </c>
-      <c r="J8" t="str">
+      <c r="H8" t="str">
         <f t="shared" si="0"/>
         <v>7,</v>
       </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>tempoChange</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="2"/>
+        <v>articulation</v>
+      </c>
       <c r="K8" t="str">
-        <f t="shared" si="1"/>
-        <v>Teaching</v>
+        <f t="shared" si="3"/>
+        <v>t_e2</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="2"/>
-        <v>Performing</v>
-      </c>
-      <c r="M8" t="str">
-        <f t="shared" si="3"/>
-        <v>tempoChange</v>
-      </c>
-      <c r="N8" t="str">
         <f t="shared" si="4"/>
-        <v>articulation</v>
-      </c>
-      <c r="O8" t="str">
-        <f t="shared" si="5"/>
-        <v>t_e2</v>
-      </c>
-      <c r="P8" t="str">
-        <f t="shared" si="6"/>
         <v>a_e1;</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
         <v>0</v>
       </c>
-      <c r="J9" t="str">
+      <c r="H9" t="str">
         <f t="shared" si="0"/>
         <v>8,</v>
       </c>
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v>tempoChange</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="2"/>
+        <v>articulation</v>
+      </c>
       <c r="K9" t="str">
-        <f t="shared" si="1"/>
-        <v>Performing</v>
+        <f t="shared" si="3"/>
+        <v>t_e2</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="2"/>
-        <v>Teaching</v>
-      </c>
-      <c r="M9" t="str">
-        <f t="shared" si="3"/>
-        <v>tempoChange</v>
-      </c>
-      <c r="N9" t="str">
         <f t="shared" si="4"/>
-        <v>articulation</v>
-      </c>
-      <c r="O9" t="str">
-        <f t="shared" si="5"/>
-        <v>t_e2</v>
-      </c>
-      <c r="P9" t="str">
-        <f t="shared" si="6"/>
         <v>a_e1;</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "Add conditions for each participant""
This reverts commit b3c7e63537c5bf9a17974c481d1c080d846cff07.
</commit_message>
<xml_diff>
--- a/script/Max/cb.xlsx
+++ b/script/Max/cb.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsukotominaga/Dropbox (Personal)/- Research/[Project]/GitHub/expert01/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsukotominaga/OneDrive - Central European University/Project/ExpertTeaching/script/Max/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18254B6C-6F0E-484E-BE8D-5C91567D5B9D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{18254B6C-6F0E-484E-BE8D-5C91567D5B9D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{267F4345-77DB-F84C-8E0D-21DD56B71286}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{52DF1984-8799-084D-A002-69ECD2D6256B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="19">
   <si>
     <t>;</t>
   </si>
@@ -64,6 +64,24 @@
   </si>
   <si>
     <t>t_e1</t>
+  </si>
+  <si>
+    <t>firstCond</t>
+  </si>
+  <si>
+    <t>firstScore</t>
+  </si>
+  <si>
+    <t>secondScore</t>
+  </si>
+  <si>
+    <t>Teaching</t>
+  </si>
+  <si>
+    <t>Performing</t>
+  </si>
+  <si>
+    <t>secondCond</t>
   </si>
 </sst>
 </file>
@@ -415,387 +433,511 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F79E29-5F9D-CD42-974F-D0505AEE028B}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="A2:E9"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>0</v>
       </c>
-      <c r="H2" t="str">
-        <f>CONCATENATE(A2,F2)</f>
+      <c r="J2" t="str">
+        <f>CONCATENATE(A2,H2)</f>
         <v>1,</v>
       </c>
-      <c r="I2" t="str">
+      <c r="K2" t="str">
         <f>B2</f>
+        <v>Teaching</v>
+      </c>
+      <c r="L2" t="str">
+        <f>C2</f>
+        <v>Performing</v>
+      </c>
+      <c r="M2" t="str">
+        <f>D2</f>
         <v>articulation</v>
       </c>
-      <c r="J2" t="str">
-        <f>C2</f>
+      <c r="N2" t="str">
+        <f>E2</f>
         <v>tempoChange</v>
       </c>
-      <c r="K2" t="str">
-        <f>D2</f>
+      <c r="O2" t="str">
+        <f>F2</f>
         <v>a_e1</v>
       </c>
-      <c r="L2" t="str">
-        <f>CONCATENATE(E2,G2)</f>
+      <c r="P2" t="str">
+        <f>CONCATENATE(G2,I2)</f>
         <v>t_e2;</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>0</v>
       </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H9" si="0">CONCATENATE(A3,F3)</f>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J9" si="0">CONCATENATE(A3,H3)</f>
         <v>2,</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I9" si="1">B3</f>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K9" si="1">B3</f>
+        <v>Performing</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L9" si="2">C3</f>
+        <v>Teaching</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M9" si="3">D3</f>
         <v>articulation</v>
       </c>
-      <c r="J3" t="str">
-        <f t="shared" ref="J3:J9" si="2">C3</f>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N9" si="4">E3</f>
         <v>tempoChange</v>
       </c>
-      <c r="K3" t="str">
-        <f t="shared" ref="K3:K9" si="3">D3</f>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O9" si="5">F3</f>
         <v>a_e1</v>
       </c>
-      <c r="L3" t="str">
-        <f t="shared" ref="L3:L9" si="4">CONCATENATE(E3,G3)</f>
+      <c r="P3" t="str">
+        <f t="shared" ref="P3:P9" si="6">CONCATENATE(G3,I3)</f>
         <v>t_e2;</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>0</v>
       </c>
-      <c r="H4" t="str">
+      <c r="J4" t="str">
         <f t="shared" si="0"/>
         <v>3,</v>
       </c>
-      <c r="I4" t="str">
+      <c r="K4" t="str">
         <f t="shared" si="1"/>
+        <v>Teaching</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="2"/>
+        <v>Performing</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="3"/>
         <v>articulation</v>
       </c>
-      <c r="J4" t="str">
-        <f t="shared" si="2"/>
+      <c r="N4" t="str">
+        <f t="shared" si="4"/>
         <v>tempoChange</v>
       </c>
-      <c r="K4" t="str">
-        <f t="shared" si="3"/>
+      <c r="O4" t="str">
+        <f t="shared" si="5"/>
         <v>a_e2</v>
       </c>
-      <c r="L4" t="str">
-        <f t="shared" si="4"/>
+      <c r="P4" t="str">
+        <f t="shared" si="6"/>
         <v>t_e1;</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>0</v>
       </c>
-      <c r="H5" t="str">
+      <c r="J5" t="str">
         <f t="shared" si="0"/>
         <v>4,</v>
       </c>
-      <c r="I5" t="str">
+      <c r="K5" t="str">
         <f t="shared" si="1"/>
+        <v>Performing</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="2"/>
+        <v>Teaching</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="3"/>
         <v>articulation</v>
       </c>
-      <c r="J5" t="str">
-        <f t="shared" si="2"/>
+      <c r="N5" t="str">
+        <f t="shared" si="4"/>
         <v>tempoChange</v>
       </c>
-      <c r="K5" t="str">
-        <f t="shared" si="3"/>
+      <c r="O5" t="str">
+        <f t="shared" si="5"/>
         <v>a_e2</v>
       </c>
-      <c r="L5" t="str">
-        <f t="shared" si="4"/>
+      <c r="P5" t="str">
+        <f t="shared" si="6"/>
         <v>t_e1;</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>0</v>
       </c>
-      <c r="H6" t="str">
+      <c r="J6" t="str">
         <f t="shared" si="0"/>
         <v>5,</v>
       </c>
-      <c r="I6" t="str">
+      <c r="K6" t="str">
         <f t="shared" si="1"/>
+        <v>Teaching</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="2"/>
+        <v>Performing</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="3"/>
         <v>tempoChange</v>
       </c>
-      <c r="J6" t="str">
-        <f t="shared" si="2"/>
+      <c r="N6" t="str">
+        <f t="shared" si="4"/>
         <v>articulation</v>
       </c>
-      <c r="K6" t="str">
-        <f t="shared" si="3"/>
+      <c r="O6" t="str">
+        <f t="shared" si="5"/>
         <v>t_e1</v>
       </c>
-      <c r="L6" t="str">
-        <f t="shared" si="4"/>
+      <c r="P6" t="str">
+        <f t="shared" si="6"/>
         <v>a_e2;</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>1</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>0</v>
       </c>
-      <c r="H7" t="str">
+      <c r="J7" t="str">
         <f t="shared" si="0"/>
         <v>6,</v>
       </c>
-      <c r="I7" t="str">
+      <c r="K7" t="str">
         <f t="shared" si="1"/>
+        <v>Performing</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="2"/>
+        <v>Teaching</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="3"/>
         <v>tempoChange</v>
       </c>
-      <c r="J7" t="str">
-        <f t="shared" si="2"/>
+      <c r="N7" t="str">
+        <f t="shared" si="4"/>
         <v>articulation</v>
       </c>
-      <c r="K7" t="str">
-        <f t="shared" si="3"/>
+      <c r="O7" t="str">
+        <f t="shared" si="5"/>
         <v>t_e1</v>
       </c>
-      <c r="L7" t="str">
-        <f t="shared" si="4"/>
+      <c r="P7" t="str">
+        <f t="shared" si="6"/>
         <v>a_e2;</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>9</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>1</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>0</v>
       </c>
-      <c r="H8" t="str">
+      <c r="J8" t="str">
         <f t="shared" si="0"/>
         <v>7,</v>
       </c>
-      <c r="I8" t="str">
+      <c r="K8" t="str">
         <f t="shared" si="1"/>
+        <v>Teaching</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="2"/>
+        <v>Performing</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="3"/>
         <v>tempoChange</v>
       </c>
-      <c r="J8" t="str">
-        <f t="shared" si="2"/>
+      <c r="N8" t="str">
+        <f t="shared" si="4"/>
         <v>articulation</v>
       </c>
-      <c r="K8" t="str">
-        <f t="shared" si="3"/>
+      <c r="O8" t="str">
+        <f t="shared" si="5"/>
         <v>t_e2</v>
       </c>
-      <c r="L8" t="str">
-        <f t="shared" si="4"/>
+      <c r="P8" t="str">
+        <f t="shared" si="6"/>
         <v>a_e1;</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>0</v>
       </c>
-      <c r="H9" t="str">
+      <c r="J9" t="str">
         <f t="shared" si="0"/>
         <v>8,</v>
       </c>
-      <c r="I9" t="str">
+      <c r="K9" t="str">
         <f t="shared" si="1"/>
+        <v>Performing</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="2"/>
+        <v>Teaching</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="3"/>
         <v>tempoChange</v>
       </c>
-      <c r="J9" t="str">
-        <f t="shared" si="2"/>
+      <c r="N9" t="str">
+        <f t="shared" si="4"/>
         <v>articulation</v>
       </c>
-      <c r="K9" t="str">
-        <f t="shared" si="3"/>
+      <c r="O9" t="str">
+        <f t="shared" si="5"/>
         <v>t_e2</v>
       </c>
-      <c r="L9" t="str">
-        <f t="shared" si="4"/>
+      <c r="P9" t="str">
+        <f t="shared" si="6"/>
         <v>a_e1;</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change the name of stimuli images
</commit_message>
<xml_diff>
--- a/script/Max/cb.xlsx
+++ b/script/Max/cb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsukotominaga/OneDrive - Central European University/Project/ExpertTeaching/script/Max/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsukotominaga/OneDrive - Central European University/Project/TeachingPiano/script/Max/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{18254B6C-6F0E-484E-BE8D-5C91567D5B9D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{267F4345-77DB-F84C-8E0D-21DD56B71286}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{18254B6C-6F0E-484E-BE8D-5C91567D5B9D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{70790A5E-329B-584B-B15B-44A1D8FB927F}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{52DF1984-8799-084D-A002-69ECD2D6256B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="17">
   <si>
     <t>;</t>
   </si>
@@ -54,18 +54,6 @@
     <t>secondStimuli</t>
   </si>
   <si>
-    <t>a_e1</t>
-  </si>
-  <si>
-    <t>t_e2</t>
-  </si>
-  <si>
-    <t>a_e2</t>
-  </si>
-  <si>
-    <t>t_e1</t>
-  </si>
-  <si>
     <t>firstCond</t>
   </si>
   <si>
@@ -82,6 +70,12 @@
   </si>
   <si>
     <t>secondCond</t>
+  </si>
+  <si>
+    <t>stim_a</t>
+  </si>
+  <si>
+    <t>stim_t</t>
   </si>
 </sst>
 </file>
@@ -436,7 +430,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="G6" sqref="G6:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -446,10 +440,10 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -458,19 +452,19 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J1" t="s">
         <v>4</v>
       </c>
       <c r="K1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
@@ -490,10 +484,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -502,10 +496,10 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
         <v>1</v>
@@ -535,11 +529,11 @@
       </c>
       <c r="O2" t="str">
         <f>F2</f>
-        <v>a_e1</v>
+        <v>stim_a</v>
       </c>
       <c r="P2" t="str">
         <f>CONCATENATE(G2,I2)</f>
-        <v>t_e2;</v>
+        <v>stim_t;</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -547,10 +541,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
@@ -559,10 +553,10 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
         <v>1</v>
@@ -592,11 +586,11 @@
       </c>
       <c r="O3" t="str">
         <f t="shared" ref="O3:O9" si="5">F3</f>
-        <v>a_e1</v>
+        <v>stim_a</v>
       </c>
       <c r="P3" t="str">
         <f t="shared" ref="P3:P9" si="6">CONCATENATE(G3,I3)</f>
-        <v>t_e2;</v>
+        <v>stim_t;</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -604,10 +598,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
@@ -616,10 +610,10 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
         <v>1</v>
@@ -649,11 +643,11 @@
       </c>
       <c r="O4" t="str">
         <f t="shared" si="5"/>
-        <v>a_e2</v>
+        <v>stim_a</v>
       </c>
       <c r="P4" t="str">
         <f t="shared" si="6"/>
-        <v>t_e1;</v>
+        <v>stim_t;</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -661,10 +655,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
@@ -673,10 +667,10 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
         <v>1</v>
@@ -706,11 +700,11 @@
       </c>
       <c r="O5" t="str">
         <f t="shared" si="5"/>
-        <v>a_e2</v>
+        <v>stim_a</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" si="6"/>
-        <v>t_e1;</v>
+        <v>stim_t;</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -718,10 +712,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -730,10 +724,10 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
         <v>1</v>
@@ -763,11 +757,11 @@
       </c>
       <c r="O6" t="str">
         <f t="shared" si="5"/>
-        <v>t_e1</v>
+        <v>stim_t</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" si="6"/>
-        <v>a_e2;</v>
+        <v>stim_a;</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -775,10 +769,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -787,10 +781,10 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s">
         <v>1</v>
@@ -820,11 +814,11 @@
       </c>
       <c r="O7" t="str">
         <f t="shared" si="5"/>
-        <v>t_e1</v>
+        <v>stim_t</v>
       </c>
       <c r="P7" t="str">
         <f t="shared" si="6"/>
-        <v>a_e2;</v>
+        <v>stim_a;</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -832,10 +826,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
@@ -844,10 +838,10 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H8" t="s">
         <v>1</v>
@@ -877,11 +871,11 @@
       </c>
       <c r="O8" t="str">
         <f t="shared" si="5"/>
-        <v>t_e2</v>
+        <v>stim_t</v>
       </c>
       <c r="P8" t="str">
         <f t="shared" si="6"/>
-        <v>a_e1;</v>
+        <v>stim_a;</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -889,10 +883,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
@@ -901,10 +895,10 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H9" t="s">
         <v>1</v>
@@ -934,11 +928,11 @@
       </c>
       <c r="O9" t="str">
         <f t="shared" si="5"/>
-        <v>t_e2</v>
+        <v>stim_t</v>
       </c>
       <c r="P9" t="str">
         <f t="shared" si="6"/>
-        <v>a_e1;</v>
+        <v>stim_a;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>